<commit_message>
Added Madrid System Extraction Logic
</commit_message>
<xml_diff>
--- a/output/2024.xlsx
+++ b/output/2024.xlsx
@@ -15355,7 +15355,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F437"/>
+  <dimension ref="A1:F742"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -23922,6 +23922,13 @@
         </is>
       </c>
     </row>
+    <row r="306">
+      <c r="E306" t="inlineStr">
+        <is>
+          <t>W. Kariuki &amp; Co. Advocates  of P. O. Box 12583 - 00400, Nairobi, Kenya</t>
+        </is>
+      </c>
+    </row>
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
@@ -27696,6 +27703,2127 @@
       <c r="F437" t="inlineStr">
         <is>
           <t>NARA 112  Corrigenda</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>6, 7 and 20</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>3</t>
         </is>
       </c>
     </row>
@@ -27711,7 +29839,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F338"/>
+  <dimension ref="A1:F499"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -37176,6 +39304,1119 @@
       <c r="F338" t="inlineStr">
         <is>
           <t>112  Corrigenda</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>3, 9, 16, 18 and 25</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>1 and 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>38</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>28</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>36</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>42</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>9</t>
         </is>
       </c>
     </row>
@@ -37191,7 +40432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F405"/>
+  <dimension ref="A1:F517"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -48867,6 +52108,790 @@
         </is>
       </c>
     </row>
+    <row r="406">
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>9 and 45</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>1 and 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>1 and 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>1 and 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>34</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>44</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>32</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing r:id="rId1"/>

</xml_diff>